<commit_message>
Parameterize main parameters in project. Misc. code improvements and clean-up.
-DN
</commit_message>
<xml_diff>
--- a/input_files/countries_for_test.xlsx
+++ b/input_files/countries_for_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\CS4269_Group4_Project1\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\CS_4269_Work\project_files\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959F2AF3-8F67-4732-BA4C-D0936E75F383}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EFD0C1-8148-4460-B6DE-3A22F5A7906B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1A7FB1F9-9FF5-41A2-805C-7AEB6DAE6997}"/>
   </bookViews>
@@ -112,14 +112,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -480,13 +480,14 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P7"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="14" max="14" width="13.33203125" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" customWidth="1"/>
+    <col min="16" max="16" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -549,11 +550,11 @@
       </c>
       <c r="C2" s="1">
         <f ca="1">SUM(PRODUCT(RANDBETWEEN(0,5), 200),1000)</f>
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">PRODUCT(SUM(PRODUCT(RANDBETWEEN(0,5), 0.15),0.2), E2)</f>
-        <v>14250</v>
+        <v>9749.9999999999982</v>
       </c>
       <c r="E2" s="1">
         <f ca="1">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
@@ -569,23 +570,23 @@
       </c>
       <c r="H2" s="1">
         <f ca="1">SUM(PRODUCT(RANDBETWEEN(0,5), 200),500)</f>
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="I2" s="1">
         <f ca="1">SUM(PRODUCT(RANDBETWEEN(0,5), 2000),12000)</f>
-        <v>16000</v>
+        <v>14000</v>
       </c>
       <c r="J2" s="1">
         <f ca="1">SUM(PRODUCT(RANDBETWEEN(0,5), 2000),12000)</f>
-        <v>18000</v>
+        <v>22000</v>
       </c>
       <c r="K2" s="1">
         <f ca="1">SUM(PRODUCT(RANDBETWEEN(0,5), 200),1000)</f>
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="L2" s="1">
         <f t="shared" ref="L2:N7" ca="1" si="0">SUM(PRODUCT(RANDBETWEEN(0,5), 200),1000)</f>
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="M2" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -593,15 +594,14 @@
       </c>
       <c r="N2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="O2" s="1">
         <f ca="1">RANDBETWEEN(0,1)</f>
         <v>1</v>
       </c>
       <c r="P2" s="1">
-        <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -610,63 +610,62 @@
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B7" ca="1" si="1">SUM(PRODUCT(RANDBETWEEN(0,5), 2000),10000)</f>
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C7" ca="1" si="2">SUM(PRODUCT(RANDBETWEEN(0,5), 200),1000)</f>
-        <v>1600</v>
+        <v>1400</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D7" ca="1" si="3">PRODUCT(SUM(PRODUCT(RANDBETWEEN(0,5), 0.15),0.2), E3)</f>
-        <v>8000</v>
+        <v>12500</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E7" ca="1" si="4">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
-        <v>10000</v>
+        <v>25000</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F7" ca="1" si="5">SUM(PRODUCT(RANDBETWEEN(5,10), 5000),10000)</f>
-        <v>55000</v>
+        <v>60000</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:H7" ca="1" si="6">SUM(PRODUCT(RANDBETWEEN(0,5), 200),500)</f>
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:J7" ca="1" si="7">SUM(PRODUCT(RANDBETWEEN(0,5), 2000),12000)</f>
-        <v>22000</v>
+        <v>18000</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>14000</v>
+        <v>20000</v>
       </c>
       <c r="K3" s="1">
         <f t="shared" ref="K3:K7" ca="1" si="8">SUM(PRODUCT(RANDBETWEEN(0,5), 200),1000)</f>
+        <v>1800</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>2000</v>
       </c>
-      <c r="L3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1600</v>
-      </c>
       <c r="M3" s="1">
         <f t="shared" ca="1" si="0"/>
         <v>2000</v>
       </c>
       <c r="N3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="O3" s="1">
         <f t="shared" ref="O3:P7" ca="1" si="9">RANDBETWEEN(0,1)</f>
         <v>1</v>
       </c>
       <c r="P3" s="1">
-        <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -675,63 +674,62 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>16000</v>
+        <v>18000</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1800</v>
+        <v>1400</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>16249.999999999998</v>
+        <v>14250</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>25000</v>
+        <v>15000</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>55000</v>
+        <v>45000</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>500</v>
+        <v>1100</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>1300</v>
+        <v>700</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>14000</v>
+        <v>12000</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>1600</v>
+        <v>1200</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2000</v>
+        <v>1400</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1800</v>
+        <v>1400</v>
       </c>
       <c r="O4" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="1">
-        <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -740,11 +738,11 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>18000</v>
+        <v>20000</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -756,27 +754,27 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>60000</v>
+        <v>45000</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>900</v>
+        <v>1100</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>14000</v>
+        <v>18000</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>18000</v>
+        <v>14000</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>1800</v>
+        <v>1000</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -784,19 +782,18 @@
       </c>
       <c r="M5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="1">
-        <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -805,27 +802,27 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>16000</v>
+        <v>18000</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>28000</v>
+        <v>6499.9999999999991</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>35000</v>
+        <v>10000</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>35000</v>
+        <v>50000</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>1100</v>
+        <v>1300</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" ca="1" si="6"/>
@@ -833,23 +830,23 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>18000</v>
+        <v>12000</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>22000</v>
+        <v>12000</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>1600</v>
+        <v>1400</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1600</v>
+        <v>1400</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -860,8 +857,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="1">
-        <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -870,63 +866,62 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10000</v>
+        <v>14000</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1000</v>
+        <v>1400</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>3000</v>
+        <v>10000</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>900</v>
+        <v>1100</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>1500</v>
+        <v>1300</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>22000</v>
+        <v>14000</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>14000</v>
+        <v>16000</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" ca="1" si="8"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1200</v>
+        <v>1600</v>
       </c>
       <c r="M7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1400</v>
+        <v>1800</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7" s="1">
-        <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>